<commit_message>
Fix legenda grafici CodeCoverage
</commit_message>
<xml_diff>
--- a/DocumentazioneEsterna/PianoDiQualifica/res/ResocontoAttivitaDiVerifica/res/metriche/grafici/qualitàProcesso/graficiProcessiPrimari.xlsx
+++ b/DocumentazioneEsterna/PianoDiQualifica/res/ResocontoAttivitaDiVerifica/res/metriche/grafici/qualitàProcesso/graficiProcessiPrimari.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\Università\Terzo anno\SWE\Progetto\Documentazione\DocumentazioneEsterna\PianoDiQualifica\res\ResocontoAttivitaDiVerifica\res\metriche\grafici\qualitàProcesso\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{751F8651-F0C3-454F-B1BE-E486B6C4DCD8}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F714E85-490B-4D12-90CD-938CE52CC98C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{5B7B37C6-A546-4C3B-BB89-60D3DA2A0238}"/>
   </bookViews>
@@ -3045,7 +3045,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{410D694D-C156-456F-BB7E-21324ECFAC13}">
   <dimension ref="C4:H73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
       <selection activeCell="L70" sqref="L70"/>
     </sheetView>
   </sheetViews>

</xml_diff>